<commit_message>
Update input data sheet file in main.py
</commit_message>
<xml_diff>
--- a/config/EBT_mapping-MASTER.xlsx
+++ b/config/EBT_mapping-MASTER.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2855F43A-5AB3-4F2B-8B6F-2A3BB880CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC48972-CBD4-4387-B7D7-6506FB3886AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E19CB741-EB2E-4E41-AFA2-705D80241AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductionByTechnologyAnnual" sheetId="4" r:id="rId1"/>
     <sheet name="TotalCapacityAnnual" sheetId="3" r:id="rId2"/>
-    <sheet name="EBT_mapping_energy" sheetId="1" state="hidden" r:id="rId3"/>
-    <sheet name="EBT_mapping_capacity" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="UseByTechnology" sheetId="5" r:id="rId3"/>
+    <sheet name="EBT_mapping_energy" sheetId="1" state="hidden" r:id="rId4"/>
+    <sheet name="EBT_mapping_capacity" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EBT_mapping_energy!$A$1:$J$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProductionByTechnologyAnnual!$A$1:$J$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EBT_mapping_energy!$A$1:$J$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProductionByTechnologyAnnual!$A$1:$J$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
     <author>Finbar Barton MAUNSELL</author>
   </authors>
   <commentList>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{CC4DC374-19C7-474B-A1F7-4A7898CB165A}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{D8C224EA-A228-407B-98CC-C2BF6CB8180B}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -65,161 +66,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-would like to rename to _no_ccs</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{678DA7C0-9509-4F01-9FDD-B4150E0C4136}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-would like to rename to gas_no_ccs</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{026051AD-55DB-44A9-8D15-EB44F2B2B4E8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-should just be pv</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{FC6124CC-BF0E-4B9D-B73A-DDEF21AB6CBD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-would like to update EBT schema to have something for this as 18_02_05_other</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E58" authorId="0" shapeId="0" xr:uid="{1B3D5BFE-6A1D-4773-BB9F-DEFD71334929}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-10_01_electricity_storage</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E59" authorId="0" shapeId="0" xr:uid="{1C87BE44-FB4A-4540-9920-EAEA18803228}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-10_01_electricity_storage</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Finbar Barton MAUNSELL</author>
-  </authors>
-  <commentList>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{D8C224EA-A228-407B-98CC-C2BF6CB8180B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 row not necessary to map I think. Check with aelx, as its not in his mappin</t>
@@ -258,7 +105,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -267,7 +114,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 this could be extrapped to 12_01_of_which_pholtaics , 12_x_other_solar. Just need to ask alex.
@@ -283,7 +130,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -292,7 +139,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 cant tell if these are supposed to be _loss instead of _own? Do we even need the or is there a aggregate being outputted by the power model?</t>
@@ -307,7 +154,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -316,7 +163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 esp unsure about these ones. Just check them</t>
@@ -331,7 +178,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -340,7 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 could be renamed to storage ?</t>
@@ -355,7 +202,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -364,7 +211,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 tehse coulors could have more accurate technologies, then could make more accurate for anyting using similar powerplant eg. For input fuels</t>
@@ -379,7 +226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSEL
 how is this different to Gas_pp?
@@ -395,7 +242,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -404,7 +251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 how is this different to lignite_PP
@@ -420,7 +267,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -429,7 +276,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 YYY is for alexs bugchecking</t>
@@ -444,7 +291,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -453,7 +300,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 why are these named different to eg POW_COAL_CHP? Is it still the same mapping? Do we need both just in case?</t>
@@ -468,7 +315,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -477,7 +324,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 guess we remove this and below in yellow? Want to double check since they are  not in the  new mapping</t>
@@ -512,7 +359,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Finbar Barton MAUNSELL</author>
@@ -548,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="209">
   <si>
     <t>x</t>
   </si>
@@ -1147,38 +994,41 @@
     <t>comment</t>
   </si>
   <si>
-    <t>own use is added to this before mapping</t>
-  </si>
-  <si>
-    <t>09_01_02_01_gasturbine</t>
-  </si>
-  <si>
-    <t>09_01_02_03_ccs</t>
-  </si>
-  <si>
-    <t>09_01_08_02_csp</t>
-  </si>
-  <si>
-    <t>09_01_08_01_utility</t>
-  </si>
-  <si>
-    <t>18_01_02_01_gasturbine</t>
-  </si>
-  <si>
-    <t>18_01_02_03_ccs</t>
-  </si>
-  <si>
-    <t>18_01_08_03_csp</t>
-  </si>
-  <si>
-    <t>18_01_08_03_utility</t>
+    <t>19_01_CHP_plants</t>
+  </si>
+  <si>
+    <t>19_01_17_electricity</t>
+  </si>
+  <si>
+    <t>POW_06_crude_oil_and_ngl</t>
+  </si>
+  <si>
+    <t>09_02_chp_plants</t>
+  </si>
+  <si>
+    <t>09_02_04_biomass</t>
+  </si>
+  <si>
+    <t>09_02_01_coal</t>
+  </si>
+  <si>
+    <t>09_02_02_gas</t>
+  </si>
+  <si>
+    <t>09_02_03_oil</t>
+  </si>
+  <si>
+    <t>These rows are included via UseByTechnology</t>
+  </si>
+  <si>
+    <t>own use is added to this before mapping. Also this will be transformed into a row with sector = 09_total_transformation in the code.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1189,26 +1039,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1228,12 +1058,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1293,6 +1137,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1303,11 +1158,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -1318,14 +1174,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1333,6 +1192,91 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1407,16 +1351,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1104901</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1431,7 +1375,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1076325" y="257175"/>
+          <a:off x="2533650" y="4524375"/>
           <a:ext cx="2333626" cy="2714625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1536,15 +1480,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2046,11 +1990,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}">
-  <dimension ref="A1:L69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}">
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,8 +2003,8 @@
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.140625" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
@@ -2133,10 +2077,13 @@
         <v>108</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>-1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2168,10 +2115,13 @@
         <v>106</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>-1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2203,10 +2153,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>-1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2238,10 +2191,13 @@
         <v>101</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>-1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2273,10 +2229,13 @@
         <v>99</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>-1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2308,10 +2267,13 @@
         <v>97</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>-1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2330,8 +2292,8 @@
       <c r="E8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>200</v>
+      <c r="F8" t="s">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
@@ -2343,10 +2305,13 @@
         <v>91</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>-1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2365,8 +2330,8 @@
       <c r="E9" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>201</v>
+      <c r="F9" t="s">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -2378,10 +2343,13 @@
         <v>91</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>-1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2413,10 +2381,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>-1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2448,10 +2419,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>-1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2483,10 +2457,13 @@
         <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>-1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2505,8 +2482,8 @@
       <c r="E13" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>203</v>
+      <c r="F13" t="s">
+        <v>0</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -2518,10 +2495,13 @@
         <v>42</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>-1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2540,8 +2520,8 @@
       <c r="E14" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>202</v>
+      <c r="F14" t="s">
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
@@ -2553,10 +2533,13 @@
         <v>196</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>-1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2588,10 +2571,13 @@
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>-1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2623,10 +2609,13 @@
         <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>-1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2658,10 +2647,13 @@
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>-1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2699,7 +2691,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L18" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2737,7 +2729,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L19" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2775,7 +2767,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L20" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2794,8 +2786,8 @@
       <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>205</v>
+      <c r="F21" t="s">
+        <v>0</v>
       </c>
       <c r="G21" t="s">
         <v>0</v>
@@ -2813,7 +2805,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L21" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,8 +2824,8 @@
       <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>204</v>
+      <c r="F22" t="s">
+        <v>0</v>
       </c>
       <c r="G22" t="s">
         <v>0</v>
@@ -2851,7 +2843,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L22" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2889,7 +2881,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L23" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2927,7 +2919,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L24" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2979,7 +2971,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L26" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3017,7 +3009,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L27" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3055,7 +3047,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L28" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3071,7 +3063,7 @@
       <c r="D29" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="s">
@@ -3093,7 +3085,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L29" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3131,7 +3123,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L30" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3151,7 +3143,7 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="G31" t="s">
         <v>0</v>
@@ -3169,7 +3161,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L31" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3207,7 +3199,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L32" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3245,7 +3237,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L33" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3391,7 +3383,7 @@
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>0</v>
@@ -4017,7 +4009,7 @@
       <c r="D58" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="12" t="s">
         <v>63</v>
       </c>
       <c r="F58" t="s">
@@ -4052,7 +4044,7 @@
       <c r="D59" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="12" t="s">
         <v>63</v>
       </c>
       <c r="F59" t="s">
@@ -4155,7 +4147,7 @@
         <v>168</v>
       </c>
       <c r="D62" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E62" t="s">
         <v>22</v>
@@ -4190,7 +4182,7 @@
         <v>168</v>
       </c>
       <c r="D63" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
@@ -4225,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="D64" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E64" t="s">
         <v>16</v>
@@ -4260,7 +4252,7 @@
         <v>168</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
         <v>195</v>
@@ -4295,7 +4287,7 @@
         <v>168</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E66" t="s">
         <v>25</v>
@@ -4321,13 +4313,34 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D67" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" t="s">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67" t="s">
+        <v>0</v>
       </c>
       <c r="J67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -4335,19 +4348,19 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="E68" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F68" t="s">
         <v>0</v>
@@ -4365,24 +4378,24 @@
         <v>1</v>
       </c>
       <c r="K68">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="D69" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="E69" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -4400,42 +4413,238 @@
         <v>1</v>
       </c>
       <c r="K69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>166</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70" t="s">
+        <v>195</v>
+      </c>
+      <c r="F70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70" t="s">
+        <v>0</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" t="s">
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" t="s">
+        <v>200</v>
+      </c>
+      <c r="F72" t="s">
+        <v>0</v>
+      </c>
+      <c r="G72" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" t="s">
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s">
+        <v>0</v>
+      </c>
+      <c r="H74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74">
         <v>-1</v>
       </c>
     </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J69" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}"/>
+  <autoFilter ref="A1:J75" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}"/>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:L1 J1:J1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:L1">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D26E25-60D0-449F-BAC1-76DB5DA98778}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G52" sqref="F52:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4446,7 +4655,7 @@
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -4469,10 +4678,13 @@
         <v>192</v>
       </c>
       <c r="H1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4494,8 +4706,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4517,8 +4732,11 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -4540,10 +4758,13 @@
       <c r="G4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
         <v>179</v>
@@ -4563,10 +4784,13 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
         <v>179</v>
@@ -4586,10 +4810,13 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>179</v>
@@ -4609,804 +4836,954 @@
       <c r="G7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>95</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>139</v>
       </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>94</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>182</v>
       </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>90</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>142</v>
       </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>88</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>141</v>
       </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>86</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>140</v>
       </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>82</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>146</v>
       </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>83</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>145</v>
       </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>80</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>148</v>
       </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>147</v>
       </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>181</v>
       </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>134</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>149</v>
       </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>138</v>
       </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>133</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>150</v>
       </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>185</v>
       </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>139</v>
       </c>
-      <c r="C22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>140</v>
       </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>141</v>
       </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>111</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>186</v>
       </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>142</v>
       </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>136</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>183</v>
       </c>
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>179</v>
       </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>137</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>184</v>
       </c>
-      <c r="C29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>49</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>181</v>
       </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>145</v>
       </c>
-      <c r="C31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>146</v>
       </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>135</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>152</v>
       </c>
-      <c r="C33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>147</v>
       </c>
-      <c r="C34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>187</v>
       </c>
-      <c r="C35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>188</v>
       </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="G37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" s="11"/>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>180</v>
       </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
-        <v>0</v>
-      </c>
-      <c r="G38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>189</v>
       </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
-        <v>0</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>132</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>190</v>
       </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>191</v>
       </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>142</v>
       </c>
-      <c r="C42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" t="b">
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5417,6 +5794,942 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DF30ED-5DFB-4467-9521-7712D6072207}">
+  <dimension ref="A1:L29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" t="s">
+        <v>196</v>
+      </c>
+      <c r="J20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J1:J29">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:L1">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908F41EA-F403-4DC0-8213-2A58D2CE82FA}">
   <dimension ref="A1:O93"/>
   <sheetViews>
@@ -9037,7 +10350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74E071D-8C7B-43E3-953F-5BFF7721AF93}">
   <dimension ref="A1:J39"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated ebt mapping master
</commit_message>
<xml_diff>
--- a/config/EBT_mapping-MASTER.xlsx
+++ b/config/EBT_mapping-MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC48972-CBD4-4387-B7D7-6506FB3886AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1F251AE-5E37-4C0C-BAA2-C86456BF205B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E19CB741-EB2E-4E41-AFA2-705D80241AD3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E19CB741-EB2E-4E41-AFA2-705D80241AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductionByTechnologyAnnual" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EBT_mapping_energy!$A$1:$J$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProductionByTechnologyAnnual!$A$1:$J$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProductionByTechnologyAnnual!$A$1:$J$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="216">
   <si>
     <t>x</t>
   </si>
@@ -1022,6 +1022,27 @@
   </si>
   <si>
     <t>own use is added to this before mapping. Also this will be transformed into a row with sector = 09_total_transformation in the code.</t>
+  </si>
+  <si>
+    <t>06_crude_oil_and_ngl</t>
+  </si>
+  <si>
+    <t>These rows are included via UseByTechnology. Plus they don’t include a specification of CHP or HP, which is needed</t>
+  </si>
+  <si>
+    <t>09_x_heat_plants</t>
+  </si>
+  <si>
+    <t>09_x_01_coal</t>
+  </si>
+  <si>
+    <t>09_x_02_gas</t>
+  </si>
+  <si>
+    <t>09_x_03_oil</t>
+  </si>
+  <si>
+    <t>09_x_04_biomass</t>
   </si>
 </sst>
 </file>
@@ -1353,13 +1374,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>581026</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1991,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}">
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2104,7 @@
         <v>-1</v>
       </c>
       <c r="L2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2121,7 +2142,7 @@
         <v>-1</v>
       </c>
       <c r="L3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2159,15 +2180,15 @@
         <v>-1</v>
       </c>
       <c r="L4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>75</v>
@@ -2185,27 +2206,24 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>-1</v>
-      </c>
       <c r="L5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>75</v>
@@ -2226,7 +2244,7 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -2235,15 +2253,15 @@
         <v>-1</v>
       </c>
       <c r="L6" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
@@ -2264,7 +2282,7 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -2273,15 +2291,15 @@
         <v>-1</v>
       </c>
       <c r="L7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>75</v>
@@ -2290,7 +2308,7 @@
         <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
@@ -2299,10 +2317,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -2311,15 +2329,15 @@
         <v>-1</v>
       </c>
       <c r="L8" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>75</v>
@@ -2349,15 +2367,15 @@
         <v>-1</v>
       </c>
       <c r="L9" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -2366,7 +2384,7 @@
         <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -2375,10 +2393,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -2387,15 +2405,15 @@
         <v>-1</v>
       </c>
       <c r="L10" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
@@ -2404,7 +2422,7 @@
         <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -2413,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
         <v>0</v>
@@ -2425,15 +2443,15 @@
         <v>-1</v>
       </c>
       <c r="L11" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>75</v>
@@ -2442,7 +2460,7 @@
         <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
         <v>0</v>
@@ -2451,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
         <v>0</v>
@@ -2463,15 +2481,15 @@
         <v>-1</v>
       </c>
       <c r="L12" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -2480,7 +2498,7 @@
         <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -2489,10 +2507,10 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -2501,15 +2519,15 @@
         <v>-1</v>
       </c>
       <c r="L13" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -2530,7 +2548,7 @@
         <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>196</v>
+        <v>42</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -2539,15 +2557,15 @@
         <v>-1</v>
       </c>
       <c r="L14" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -2556,7 +2574,7 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -2565,10 +2583,10 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -2577,15 +2595,15 @@
         <v>-1</v>
       </c>
       <c r="L15" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
@@ -2594,7 +2612,7 @@
         <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -2603,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
         <v>0</v>
@@ -2615,15 +2633,15 @@
         <v>-1</v>
       </c>
       <c r="L16" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>75</v>
@@ -2632,7 +2650,7 @@
         <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -2641,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I17" t="s">
         <v>0</v>
@@ -2653,24 +2671,24 @@
         <v>-1</v>
       </c>
       <c r="L17" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
         <v>0</v>
@@ -2679,24 +2697,24 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>277.77800000000002</v>
+        <v>-1</v>
       </c>
       <c r="L18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -2705,10 +2723,10 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
         <v>0</v>
@@ -2734,7 +2752,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -2743,10 +2761,10 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
@@ -2772,7 +2790,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -2781,10 +2799,10 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
@@ -2810,7 +2828,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2848,7 +2866,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -2860,7 +2878,7 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
         <v>0</v>
@@ -2886,7 +2904,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -2898,7 +2916,7 @@
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
         <v>0</v>
@@ -2924,59 +2942,59 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>0</v>
+      </c>
       <c r="J25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>277.77800000000002</v>
+      </c>
+      <c r="L25" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>0</v>
-      </c>
       <c r="J26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>277.77800000000002</v>
-      </c>
-      <c r="L26" t="s">
-        <v>208</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -2985,10 +3003,10 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
         <v>0</v>
@@ -3014,7 +3032,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -3023,10 +3041,10 @@
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
         <v>0</v>
@@ -3052,7 +3070,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -3061,10 +3079,10 @@
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
         <v>0</v>
@@ -3090,7 +3108,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -3099,10 +3117,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="F30" t="s">
         <v>0</v>
@@ -3128,7 +3146,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -3140,7 +3158,7 @@
         <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -3166,7 +3184,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -3175,10 +3193,10 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
         <v>0</v>
@@ -3204,7 +3222,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -3213,10 +3231,10 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F33" t="s">
         <v>0</v>
@@ -3241,22 +3259,46 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>1</v>
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>1</v>
+        <v>277.77800000000002</v>
+      </c>
+      <c r="L34" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>1</v>
@@ -3270,56 +3312,35 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>0</v>
+      <c r="B37" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="J37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
-        <v>277.77800000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -3334,7 +3355,7 @@
         <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G38" t="s">
         <v>0</v>
@@ -3353,69 +3374,69 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" t="s">
+        <v>194</v>
+      </c>
+      <c r="G39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>277.77800000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="J39" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>0</v>
-      </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>277.77800000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s">
         <v>0</v>
@@ -3433,24 +3454,24 @@
         <v>1</v>
       </c>
       <c r="K41">
-        <v>-1</v>
+        <v>277.77800000000002</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="F42" t="s">
         <v>0</v>
@@ -3473,7 +3494,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
         <v>66</v>
@@ -3508,7 +3529,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>66</v>
@@ -3543,7 +3564,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -3578,7 +3599,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>66</v>
@@ -3613,7 +3634,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>66</v>
@@ -3648,7 +3669,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
@@ -3683,7 +3704,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
@@ -3718,7 +3739,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
@@ -3753,7 +3774,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
         <v>66</v>
@@ -3788,7 +3809,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
@@ -3823,7 +3844,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
@@ -3858,7 +3879,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
@@ -3893,7 +3914,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
         <v>66</v>
@@ -3928,7 +3949,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
@@ -3963,7 +3984,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B57" t="s">
         <v>66</v>
@@ -3998,7 +4019,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
@@ -4009,7 +4030,7 @@
       <c r="D58" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" t="s">
         <v>63</v>
       </c>
       <c r="F58" t="s">
@@ -4033,7 +4054,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
         <v>66</v>
@@ -4068,7 +4089,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
         <v>66</v>
@@ -4079,7 +4100,7 @@
       <c r="D60" t="s">
         <v>64</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="12" t="s">
         <v>63</v>
       </c>
       <c r="F60" t="s">
@@ -4103,7 +4124,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
@@ -4138,19 +4159,19 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C62" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s">
-        <v>199</v>
+        <v>64</v>
       </c>
       <c r="E62" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F62" t="s">
         <v>0</v>
@@ -4159,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I62" t="s">
         <v>0</v>
@@ -4168,12 +4189,12 @@
         <v>1</v>
       </c>
       <c r="K62">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
@@ -4185,7 +4206,7 @@
         <v>199</v>
       </c>
       <c r="E63" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F63" t="s">
         <v>0</v>
@@ -4208,7 +4229,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
@@ -4220,7 +4241,7 @@
         <v>199</v>
       </c>
       <c r="E64" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F64" t="s">
         <v>0</v>
@@ -4243,7 +4264,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
@@ -4255,7 +4276,7 @@
         <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="F65" t="s">
         <v>0</v>
@@ -4278,7 +4299,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
@@ -4290,7 +4311,7 @@
         <v>199</v>
       </c>
       <c r="E66" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="F66" t="s">
         <v>0</v>
@@ -4313,7 +4334,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
@@ -4322,10 +4343,10 @@
         <v>168</v>
       </c>
       <c r="D67" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E67" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F67" t="s">
         <v>0</v>
@@ -4348,7 +4369,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
@@ -4360,7 +4381,7 @@
         <v>169</v>
       </c>
       <c r="E68" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F68" t="s">
         <v>0</v>
@@ -4383,7 +4404,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
@@ -4395,7 +4416,7 @@
         <v>169</v>
       </c>
       <c r="E69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -4418,7 +4439,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
@@ -4430,7 +4451,7 @@
         <v>169</v>
       </c>
       <c r="E70" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="F70" t="s">
         <v>0</v>
@@ -4453,7 +4474,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B71" t="s">
         <v>4</v>
@@ -4465,7 +4486,7 @@
         <v>169</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="F71" t="s">
         <v>0</v>
@@ -4488,7 +4509,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -4500,7 +4521,7 @@
         <v>169</v>
       </c>
       <c r="E72" t="s">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="F72" t="s">
         <v>0</v>
@@ -4523,13 +4544,34 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E73" t="s">
+        <v>200</v>
+      </c>
+      <c r="F73" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>0</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73" t="s">
+        <v>0</v>
       </c>
       <c r="J73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -4540,34 +4582,13 @@
         <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>68</v>
-      </c>
-      <c r="C74" t="s">
-        <v>65</v>
-      </c>
-      <c r="D74" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" t="s">
-        <v>0</v>
-      </c>
-      <c r="F74" t="s">
-        <v>0</v>
-      </c>
-      <c r="G74" t="s">
-        <v>0</v>
-      </c>
-      <c r="H74" t="s">
-        <v>4</v>
-      </c>
-      <c r="I74" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K74">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -4575,16 +4596,16 @@
         <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
         <v>65</v>
       </c>
       <c r="D75" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E75" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="F75" t="s">
         <v>0</v>
@@ -4605,14 +4626,49 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" t="s">
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
+        <v>0</v>
+      </c>
+      <c r="H76" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76" t="s">
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J75" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}"/>
-  <conditionalFormatting sqref="C18">
+  <autoFilter ref="A1:J76" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}"/>
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C28">
     <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4641,10 +4697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D26E25-60D0-449F-BAC1-76DB5DA98778}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G52" sqref="F52:G52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,10 +5184,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>201</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -5146,7 +5202,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -5154,10 +5210,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -5180,10 +5236,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -5206,10 +5262,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -5232,10 +5288,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -5258,10 +5314,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
@@ -5284,10 +5340,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -5310,10 +5366,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
@@ -5328,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -5336,10 +5392,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
@@ -5354,7 +5410,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -5362,10 +5418,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
@@ -5388,10 +5444,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
@@ -5414,10 +5470,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -5440,10 +5496,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -5466,10 +5522,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -5492,10 +5548,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -5518,10 +5574,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -5544,10 +5600,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
@@ -5570,10 +5626,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
@@ -5596,10 +5652,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
@@ -5622,11 +5678,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>0</v>
+      </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -5634,23 +5704,9 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B39" s="11"/>
       <c r="G39" t="b">
         <v>0</v>
       </c>
@@ -5660,10 +5716,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -5686,10 +5742,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -5704,7 +5760,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -5712,53 +5768,79 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>70</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>191</v>
       </c>
-      <c r="C42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>142</v>
       </c>
-      <c r="C43" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>0</v>
-      </c>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43">
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44">
         <v>1</v>
       </c>
     </row>
@@ -5795,10 +5877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DF30ED-5DFB-4467-9521-7712D6072207}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6130,10 +6212,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -6142,7 +6224,7 @@
         <v>202</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -6151,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="I10" t="s">
         <v>0</v>
@@ -6165,19 +6247,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -6186,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
         <v>0</v>
@@ -6200,10 +6282,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>75</v>
@@ -6212,7 +6294,7 @@
         <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
         <v>0</v>
@@ -6221,10 +6303,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="J12" s="13" t="b">
         <v>1</v>
@@ -6238,7 +6320,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -6259,7 +6341,7 @@
         <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J13" s="13" t="b">
         <v>1</v>
@@ -6273,7 +6355,7 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -6291,10 +6373,10 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="J14" s="13" t="b">
         <v>1</v>
@@ -6305,10 +6387,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -6317,7 +6399,7 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -6326,10 +6408,10 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="I15" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="J15" s="13" t="b">
         <v>1</v>
@@ -6340,10 +6422,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
@@ -6352,7 +6434,7 @@
         <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -6361,10 +6443,10 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="J16" s="13" t="b">
         <v>1</v>
@@ -6375,10 +6457,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
         <v>75</v>
@@ -6387,7 +6469,7 @@
         <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -6396,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="I17" t="s">
         <v>0</v>
@@ -6410,10 +6492,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>75</v>
@@ -6422,7 +6504,7 @@
         <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
         <v>0</v>
@@ -6431,7 +6513,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
@@ -6445,10 +6527,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>75</v>
@@ -6457,7 +6539,7 @@
         <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
         <v>0</v>
@@ -6466,7 +6548,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="I19" t="s">
         <v>0</v>
@@ -6480,10 +6562,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
@@ -6492,7 +6574,7 @@
         <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
@@ -6501,10 +6583,10 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="J20" s="13" t="b">
         <v>1</v>
@@ -6515,21 +6597,45 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" t="s">
+        <v>196</v>
       </c>
       <c r="J21" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J22" s="13" t="b">
         <v>0</v>
@@ -6537,42 +6643,18 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>71</v>
-      </c>
-      <c r="I23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
@@ -6607,64 +6689,88 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>0</v>
       </c>
       <c r="J25" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="J26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" t="s">
+        <v>42</v>
       </c>
       <c r="J27" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
@@ -6675,41 +6781,577 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>91</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>75</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>74</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>92</v>
       </c>
-      <c r="F29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
         <v>18</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>91</v>
       </c>
-      <c r="J29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29">
+      <c r="J30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30">
         <v>-1</v>
       </c>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" t="s">
+        <v>211</v>
+      </c>
+      <c r="E31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" t="s">
+        <v>108</v>
+      </c>
+      <c r="J35" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" t="s">
+        <v>212</v>
+      </c>
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>211</v>
+      </c>
+      <c r="E37" t="s">
+        <v>212</v>
+      </c>
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
+        <v>103</v>
+      </c>
+      <c r="I37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" t="s">
+        <v>214</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>211</v>
+      </c>
+      <c r="E40" t="s">
+        <v>214</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" t="s">
+        <v>211</v>
+      </c>
+      <c r="E41" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>209</v>
+      </c>
+      <c r="I41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>101</v>
+      </c>
+      <c r="J42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>99</v>
+      </c>
+      <c r="J43" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>97</v>
+      </c>
+      <c r="J44" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>209</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>209</v>
+      </c>
+      <c r="I45" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J1:J29">
+  <conditionalFormatting sqref="J1:J45">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
minor changes in names to bring them in line with EGEDA
</commit_message>
<xml_diff>
--- a/config/EBT_mapping-MASTER.xlsx
+++ b/config/EBT_mapping-MASTER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\power-model\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1F251AE-5E37-4C0C-BAA2-C86456BF205B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11A5C65-8748-4BAB-B155-32B7735881FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E19CB741-EB2E-4E41-AFA2-705D80241AD3}"/>
+    <workbookView xWindow="2775" yWindow="855" windowWidth="24570" windowHeight="14625" xr2:uid="{E19CB741-EB2E-4E41-AFA2-705D80241AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductionByTechnologyAnnual" sheetId="4" r:id="rId1"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="215">
   <si>
     <t>x</t>
   </si>
@@ -976,12 +976,6 @@
     <t>TO_USE</t>
   </si>
   <si>
-    <t>18_01_09_02_wind_offshore</t>
-  </si>
-  <si>
-    <t>18_01_09_01_wind_onshore</t>
-  </si>
-  <si>
     <t>19_01_05_others</t>
   </si>
   <si>
@@ -994,9 +988,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>19_01_CHP_plants</t>
-  </si>
-  <si>
     <t>19_01_17_electricity</t>
   </si>
   <si>
@@ -1043,6 +1034,12 @@
   </si>
   <si>
     <t>09_x_04_biomass</t>
+  </si>
+  <si>
+    <t>18_01_09_02_offshore</t>
+  </si>
+  <si>
+    <t>18_01_09_01_onshore</t>
   </si>
 </sst>
 </file>
@@ -2014,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABF96D6-2077-4AE8-A24F-6F8A1C74C43F}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,10 +2060,10 @@
         <v>192</v>
       </c>
       <c r="K1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2104,7 +2101,7 @@
         <v>-1</v>
       </c>
       <c r="L2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2142,7 +2139,7 @@
         <v>-1</v>
       </c>
       <c r="L3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2180,15 +2177,15 @@
         <v>-1</v>
       </c>
       <c r="L4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
         <v>75</v>
@@ -2206,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I5" t="s">
         <v>0</v>
@@ -2215,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2253,7 +2250,7 @@
         <v>-1</v>
       </c>
       <c r="L6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2291,7 +2288,7 @@
         <v>-1</v>
       </c>
       <c r="L7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2329,7 +2326,7 @@
         <v>-1</v>
       </c>
       <c r="L8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2367,7 +2364,7 @@
         <v>-1</v>
       </c>
       <c r="L9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2405,7 +2402,7 @@
         <v>-1</v>
       </c>
       <c r="L10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2443,7 +2440,7 @@
         <v>-1</v>
       </c>
       <c r="L11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2481,7 +2478,7 @@
         <v>-1</v>
       </c>
       <c r="L12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2519,7 +2516,7 @@
         <v>-1</v>
       </c>
       <c r="L13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2557,7 +2554,7 @@
         <v>-1</v>
       </c>
       <c r="L14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,7 +2583,7 @@
         <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -2595,7 +2592,7 @@
         <v>-1</v>
       </c>
       <c r="L15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2633,7 +2630,7 @@
         <v>-1</v>
       </c>
       <c r="L16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2671,7 +2668,7 @@
         <v>-1</v>
       </c>
       <c r="L17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2709,7 +2706,7 @@
         <v>-1</v>
       </c>
       <c r="L18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2747,7 +2744,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2785,7 +2782,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2823,7 +2820,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2861,7 +2858,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L22" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2899,7 +2896,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2937,7 +2934,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2975,7 +2972,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L25" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3027,7 +3024,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L27" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3065,7 +3062,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3103,7 +3100,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L29" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3141,7 +3138,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L30" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3179,7 +3176,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3217,7 +3214,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L32" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3255,7 +3252,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3293,7 +3290,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="L34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3355,7 +3352,7 @@
         <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="G38" t="s">
         <v>0</v>
@@ -3390,7 +3387,7 @@
         <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="G39" t="s">
         <v>0</v>
@@ -4200,10 +4197,10 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
         <v>22</v>
@@ -4235,10 +4232,10 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
@@ -4270,10 +4267,10 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
         <v>16</v>
@@ -4305,13 +4302,13 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F66" t="s">
         <v>0</v>
@@ -4340,10 +4337,10 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -4375,7 +4372,7 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D68" t="s">
         <v>169</v>
@@ -4410,7 +4407,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D69" t="s">
         <v>169</v>
@@ -4445,7 +4442,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
         <v>169</v>
@@ -4480,13 +4477,13 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D71" t="s">
         <v>169</v>
       </c>
       <c r="E71" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F71" t="s">
         <v>0</v>
@@ -4515,7 +4512,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D72" t="s">
         <v>169</v>
@@ -4550,13 +4547,13 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="D73" t="s">
         <v>169</v>
       </c>
       <c r="E73" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F73" t="s">
         <v>0</v>
@@ -4734,10 +4731,10 @@
         <v>192</v>
       </c>
       <c r="H1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4820,7 +4817,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
         <v>179</v>
@@ -5184,7 +5181,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
         <v>179</v>
@@ -5879,8 +5876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DF30ED-5DFB-4467-9521-7712D6072207}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5924,10 +5921,10 @@
         <v>192</v>
       </c>
       <c r="K1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5941,10 +5938,10 @@
         <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -5976,10 +5973,10 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -6011,10 +6008,10 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -6046,10 +6043,10 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -6081,10 +6078,10 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" t="s">
         <v>202</v>
-      </c>
-      <c r="E6" t="s">
-        <v>205</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -6116,10 +6113,10 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -6151,10 +6148,10 @@
         <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
@@ -6186,10 +6183,10 @@
         <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -6215,25 +6212,25 @@
         <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
         <v>206</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>209</v>
       </c>
       <c r="I10" t="s">
         <v>0</v>
@@ -6256,7 +6253,7 @@
         <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -6621,7 +6618,7 @@
         <v>43</v>
       </c>
       <c r="I21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J21" s="13" t="b">
         <v>1</v>
@@ -6836,10 +6833,10 @@
         <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -6871,7 +6868,7 @@
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
@@ -6906,10 +6903,10 @@
         <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F33" t="s">
         <v>0</v>
@@ -6941,7 +6938,7 @@
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E34" t="s">
         <v>0</v>
@@ -6976,10 +6973,10 @@
         <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F35" t="s">
         <v>0</v>
@@ -7011,10 +7008,10 @@
         <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E36" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F36" t="s">
         <v>0</v>
@@ -7046,10 +7043,10 @@
         <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F37" t="s">
         <v>0</v>
@@ -7081,10 +7078,10 @@
         <v>75</v>
       </c>
       <c r="D38" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38" t="s">
         <v>211</v>
-      </c>
-      <c r="E38" t="s">
-        <v>214</v>
       </c>
       <c r="F38" t="s">
         <v>0</v>
@@ -7116,10 +7113,10 @@
         <v>75</v>
       </c>
       <c r="D39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E39" t="s">
         <v>211</v>
-      </c>
-      <c r="E39" t="s">
-        <v>214</v>
       </c>
       <c r="F39" t="s">
         <v>0</v>
@@ -7151,10 +7148,10 @@
         <v>75</v>
       </c>
       <c r="D40" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" t="s">
         <v>211</v>
-      </c>
-      <c r="E40" t="s">
-        <v>214</v>
       </c>
       <c r="F40" t="s">
         <v>0</v>
@@ -7180,17 +7177,17 @@
         <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
         <v>75</v>
       </c>
       <c r="D41" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" t="s">
         <v>211</v>
       </c>
-      <c r="E41" t="s">
-        <v>214</v>
-      </c>
       <c r="F41" t="s">
         <v>0</v>
       </c>
@@ -7198,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I41" t="s">
         <v>0</v>
@@ -7320,7 +7317,7 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C45" t="s">
         <v>75</v>
@@ -7338,7 +7335,7 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I45" t="s">
         <v>0</v>

</xml_diff>